<commit_message>
Updated tasks and contact info(github).
</commit_message>
<xml_diff>
--- a/TeamOrangeTasks.xlsx
+++ b/TeamOrangeTasks.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27322"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-5020" yWindow="-21220" windowWidth="28800" windowHeight="13540" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Contacts" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="61">
   <si>
     <t>Scott Bushyhead</t>
   </si>
@@ -167,13 +167,52 @@
   </si>
   <si>
     <t>Account: NerdboyTyler</t>
+  </si>
+  <si>
+    <t>T01_Orange</t>
+  </si>
+  <si>
+    <t>Complete Project</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Completed</t>
+  </si>
+  <si>
+    <t>Assigned</t>
+  </si>
+  <si>
+    <t>Splash Screen</t>
+  </si>
+  <si>
+    <t>Level 1 Ideas</t>
+  </si>
+  <si>
+    <t>Level 2 Ideas</t>
+  </si>
+  <si>
+    <t>Level 3 Ideas</t>
+  </si>
+  <si>
+    <t>NerdboyTyler</t>
+  </si>
+  <si>
+    <t>ammarhz</t>
+  </si>
+  <si>
+    <t>NerdAlert58</t>
+  </si>
+  <si>
+    <t>Account: ammarhz</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -211,6 +250,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -229,7 +275,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="10">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -240,15 +286,18 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="10">
+  <cellStyles count="12">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -257,6 +306,8 @@
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -539,7 +590,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -553,11 +604,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
@@ -595,8 +646,8 @@
       <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>7</v>
+      <c r="F3" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -615,6 +666,9 @@
       <c r="E4" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="F4" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" t="s">
@@ -652,13 +706,16 @@
       <c r="E6" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="F6" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
@@ -689,7 +746,7 @@
     <hyperlink ref="E5" r:id="rId10"/>
     <hyperlink ref="D6" r:id="rId11"/>
     <hyperlink ref="E6" r:id="rId12"/>
-    <hyperlink ref="F3" r:id="rId13"/>
+    <hyperlink ref="F3" r:id="rId13" display="bushyhead@gmail.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
@@ -703,15 +760,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J6"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
@@ -759,22 +816,25 @@
       <c r="B2" t="s">
         <v>29</v>
       </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
       <c r="D2" t="s">
         <v>30</v>
       </c>
       <c r="E2" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="4">
+      <c r="F2" s="3">
         <v>42620</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="3">
         <v>42620</v>
       </c>
       <c r="H2">
         <v>4</v>
       </c>
-      <c r="I2" s="4">
+      <c r="I2" s="3">
         <v>42620</v>
       </c>
       <c r="J2" t="s">
@@ -788,19 +848,22 @@
       <c r="B3" t="s">
         <v>38</v>
       </c>
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
       <c r="D3" t="s">
         <v>30</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>42620</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
         <v>42627</v>
       </c>
       <c r="H3">
         <v>1</v>
       </c>
-      <c r="I3" s="4">
+      <c r="I3" s="3">
         <v>42620</v>
       </c>
       <c r="J3" t="s">
@@ -814,19 +877,22 @@
       <c r="B4" t="s">
         <v>39</v>
       </c>
+      <c r="C4" t="s">
+        <v>51</v>
+      </c>
       <c r="D4" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>42620</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>42627</v>
       </c>
       <c r="H4">
         <v>1</v>
       </c>
-      <c r="I4" s="4">
+      <c r="I4" s="3">
         <v>42620</v>
       </c>
       <c r="J4" t="s">
@@ -840,19 +906,22 @@
       <c r="B5" t="s">
         <v>39</v>
       </c>
+      <c r="C5" t="s">
+        <v>51</v>
+      </c>
       <c r="D5" t="s">
         <v>40</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>42620</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>42627</v>
       </c>
       <c r="H5">
         <v>1</v>
       </c>
-      <c r="I5" s="4">
+      <c r="I5" s="3">
         <v>42620</v>
       </c>
       <c r="J5" t="s">
@@ -866,20 +935,89 @@
       <c r="B6" t="s">
         <v>39</v>
       </c>
+      <c r="C6" t="s">
+        <v>52</v>
+      </c>
       <c r="D6" t="s">
         <v>41</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>42620</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <v>42627</v>
       </c>
       <c r="H6">
         <v>1</v>
       </c>
+      <c r="I6" s="3">
+        <v>42622</v>
+      </c>
+      <c r="J6" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="3">
+        <v>42620</v>
+      </c>
+      <c r="G7" s="3">
+        <v>42640</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
     </row>
   </sheetData>
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576">
+      <formula1>"Assigned,Started,In Progress,On Hold,Completed"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
Uploading Scott's version of HW4
</commit_message>
<xml_diff>
--- a/TeamOrangeTasks.xlsx
+++ b/TeamOrangeTasks.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="65">
   <si>
     <t>Scott Bushyhead</t>
   </si>
@@ -109,9 +109,6 @@
     <t>Start Date</t>
   </si>
   <si>
-    <t>Estimated hours</t>
-  </si>
-  <si>
     <t>Questions</t>
   </si>
   <si>
@@ -172,9 +169,6 @@
     <t>T01_Orange</t>
   </si>
   <si>
-    <t>Complete Project</t>
-  </si>
-  <si>
     <t>In Progress</t>
   </si>
   <si>
@@ -206,6 +200,24 @@
   </si>
   <si>
     <t>Account: ammarhz</t>
+  </si>
+  <si>
+    <t>Testing Level 1</t>
+  </si>
+  <si>
+    <t>Testing Level 2</t>
+  </si>
+  <si>
+    <t>Testing Level 3</t>
+  </si>
+  <si>
+    <t>Complete 1st Team Project</t>
+  </si>
+  <si>
+    <t>Design</t>
+  </si>
+  <si>
+    <t>Estimated Hours</t>
   </si>
 </sst>
 </file>
@@ -258,15 +270,39 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF008000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6600"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -274,8 +310,23 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="12">
+  <cellStyleXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -288,16 +339,25 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="12">
+  <cellStyles count="13">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -308,6 +368,7 @@
     <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -579,7 +640,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -590,7 +651,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -604,11 +665,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
@@ -627,7 +688,7 @@
         <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -647,7 +708,7 @@
         <v>7</v>
       </c>
       <c r="F3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -667,7 +728,7 @@
         <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -687,7 +748,7 @@
         <v>20</v>
       </c>
       <c r="F5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -707,15 +768,15 @@
         <v>22</v>
       </c>
       <c r="F6" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:6">
       <c r="A8" t="s">
@@ -760,260 +821,369 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J11"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="95.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" style="4"/>
+    <col min="4" max="4" width="6.83203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.1640625" style="4"/>
+    <col min="7" max="7" width="15.33203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="95.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="11.1640625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="A1" t="s">
+      <c r="A1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="D1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" t="s">
-        <v>26</v>
-      </c>
-      <c r="F1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" t="s">
+      <c r="H1" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" s="7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="I1" t="s">
+      <c r="C2" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="9">
+        <v>42620</v>
+      </c>
+      <c r="G2" s="9">
+        <v>42620</v>
+      </c>
+      <c r="H2" s="6">
+        <v>4</v>
+      </c>
+      <c r="I2" s="9">
+        <v>42620</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10">
+      <c r="A3" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="9">
+        <v>42620</v>
+      </c>
+      <c r="G3" s="9">
+        <v>42627</v>
+      </c>
+      <c r="H3" s="6">
+        <v>1</v>
+      </c>
+      <c r="I3" s="9">
+        <v>42620</v>
+      </c>
+      <c r="J3" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="J1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B2" t="s">
+    </row>
+    <row r="4" spans="1:10">
+      <c r="A4" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C4" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="9">
+        <v>42620</v>
+      </c>
+      <c r="G4" s="9">
+        <v>42627</v>
+      </c>
+      <c r="H4" s="6">
+        <v>1</v>
+      </c>
+      <c r="I4" s="9">
+        <v>42620</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
+      <c r="A5" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E5" s="6"/>
+      <c r="F5" s="9">
+        <v>42620</v>
+      </c>
+      <c r="G5" s="9">
+        <v>42627</v>
+      </c>
+      <c r="H5" s="6">
+        <v>1</v>
+      </c>
+      <c r="I5" s="9">
+        <v>42620</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
+      <c r="A6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="6"/>
+      <c r="F6" s="9">
+        <v>42620</v>
+      </c>
+      <c r="G6" s="9">
+        <v>42627</v>
+      </c>
+      <c r="H6" s="6">
+        <v>1</v>
+      </c>
+      <c r="I6" s="9">
+        <v>42622</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
+      <c r="A7" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" s="3">
+      <c r="E7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="9">
         <v>42620</v>
       </c>
-      <c r="G2" s="3">
-        <v>42620</v>
-      </c>
-      <c r="H2">
-        <v>4</v>
-      </c>
-      <c r="I2" s="3">
-        <v>42620</v>
-      </c>
-      <c r="J2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10">
-      <c r="A3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="G7" s="9">
+        <v>42640</v>
+      </c>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:10">
+      <c r="A8" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="9"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="1:10">
+      <c r="A9" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D3" t="s">
-        <v>30</v>
-      </c>
-      <c r="F3" s="3">
-        <v>42620</v>
-      </c>
-      <c r="G3" s="3">
-        <v>42627</v>
-      </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-      <c r="I3" s="3">
-        <v>42620</v>
-      </c>
-      <c r="J3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10">
-      <c r="A4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B4" t="s">
-        <v>39</v>
-      </c>
-      <c r="C4" t="s">
-        <v>51</v>
-      </c>
-      <c r="D4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F4" s="3">
-        <v>42620</v>
-      </c>
-      <c r="G4" s="3">
-        <v>42627</v>
-      </c>
-      <c r="H4">
-        <v>1</v>
-      </c>
-      <c r="I4" s="3">
-        <v>42620</v>
-      </c>
-      <c r="J4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10">
-      <c r="A5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B5" t="s">
-        <v>39</v>
-      </c>
-      <c r="C5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D5" t="s">
-        <v>40</v>
-      </c>
-      <c r="F5" s="3">
-        <v>42620</v>
-      </c>
-      <c r="G5" s="3">
-        <v>42627</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5" s="3">
-        <v>42620</v>
-      </c>
-      <c r="J5" t="s">
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+    </row>
+    <row r="10" spans="1:10">
+      <c r="A10" s="13" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="6" spans="1:10">
-      <c r="A6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B10" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="D6" t="s">
-        <v>41</v>
-      </c>
-      <c r="F6" s="3">
-        <v>42620</v>
-      </c>
-      <c r="G6" s="3">
-        <v>42627</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6" s="3">
-        <v>42622</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+    </row>
+    <row r="11" spans="1:10">
+      <c r="A11" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+    </row>
+    <row r="12" spans="1:10">
+      <c r="A12" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+    </row>
+    <row r="13" spans="1:10">
+      <c r="A13" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+    </row>
+    <row r="14" spans="1:10">
+      <c r="A14" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="6" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="A7" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F7" s="3">
-        <v>42620</v>
-      </c>
-      <c r="G7" s="3">
-        <v>42640</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="A8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10">
-      <c r="A9" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" t="s">
-        <v>56</v>
-      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+    </row>
+    <row r="15" spans="1:10">
+      <c r="A15" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
     </row>
   </sheetData>
-  <dataValidations disablePrompts="1" count="1">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576">
       <formula1>"Assigned,Started,In Progress,On Hold,Completed"</formula1>
     </dataValidation>

</xml_diff>

<commit_message>
Updated tasks and Puzzle.swift -Scott
</commit_message>
<xml_diff>
--- a/TeamOrangeTasks.xlsx
+++ b/TeamOrangeTasks.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="74">
   <si>
     <t>Scott Bushyhead</t>
   </si>
@@ -232,16 +232,19 @@
     <t>Level 3 Ideas 5X5</t>
   </si>
   <si>
-    <t>Needs review/acceptance by team</t>
-  </si>
-  <si>
-    <t>Method: Array_Modify</t>
-  </si>
-  <si>
     <t>Background Layout</t>
   </si>
   <si>
     <t>Levels Layout</t>
+  </si>
+  <si>
+    <t>Splash Screen Button update</t>
+  </si>
+  <si>
+    <t>Method: modArray</t>
+  </si>
+  <si>
+    <t>Accepted</t>
   </si>
 </sst>
 </file>
@@ -350,9 +353,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="14">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -382,7 +388,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="14">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
@@ -395,6 +401,9 @@
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="15" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -666,7 +675,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -849,16 +858,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
+      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="14.5" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="11.1640625" style="3"/>
     <col min="4" max="4" width="6.83203125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.1640625" style="3" bestFit="1" customWidth="1"/>
@@ -1127,7 +1136,7 @@
         <v>42631</v>
       </c>
       <c r="J9" s="5" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:10">
@@ -1137,8 +1146,8 @@
       <c r="B10" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>50</v>
+      <c r="C10" s="9" t="s">
+        <v>49</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>39</v>
@@ -1153,7 +1162,9 @@
       <c r="H10" s="5">
         <v>2</v>
       </c>
-      <c r="I10" s="5"/>
+      <c r="I10" s="8">
+        <v>42633</v>
+      </c>
       <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10">
@@ -1209,19 +1220,25 @@
         <v>47</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C13" s="5" t="s">
-        <v>50</v>
+        <v>72</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>49</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>29</v>
       </c>
       <c r="E13" s="5"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
+      <c r="F13" s="8">
+        <v>42631</v>
+      </c>
+      <c r="G13" s="8">
+        <v>42636</v>
+      </c>
       <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
+      <c r="I13" s="8">
+        <v>42633</v>
+      </c>
       <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10">
@@ -1229,7 +1246,7 @@
         <v>47</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>50</v>
@@ -1238,8 +1255,12 @@
         <v>39</v>
       </c>
       <c r="E14" s="5"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
+      <c r="F14" s="8">
+        <v>42631</v>
+      </c>
+      <c r="G14" s="8">
+        <v>42636</v>
+      </c>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
@@ -1249,31 +1270,47 @@
         <v>47</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>50</v>
+        <v>70</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>49</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>40</v>
       </c>
       <c r="E15" s="5"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
+      <c r="F15" s="8">
+        <v>42631</v>
+      </c>
+      <c r="G15" s="8">
+        <v>42636</v>
+      </c>
       <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
+      <c r="I15" s="8">
+        <v>42633</v>
+      </c>
       <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10">
       <c r="A16" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="B16" s="5"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
+      <c r="B16" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>40</v>
+      </c>
       <c r="E16" s="5"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
+      <c r="F16" s="8">
+        <v>42631</v>
+      </c>
+      <c r="G16" s="8">
+        <v>42636</v>
+      </c>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>

</xml_diff>